<commit_message>
make all trees have same date
</commit_message>
<xml_diff>
--- a/data/tle/2020-02-12_CEI.xlsx
+++ b/data/tle/2020-02-12_CEI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrcunning/Projects/bsrte/data/tle/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{003B71EF-42C1-6644-BBBD-B1D37C7B44B5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C41C288-DE28-6543-9B0E-2D3CD541471C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="940" windowWidth="27640" windowHeight="16000" xr2:uid="{95812F95-F459-FF47-9666-98D8637D2352}"/>
   </bookViews>
@@ -881,19 +881,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1211,7 +1211,7 @@
   <dimension ref="A1:AJ1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AL3" sqref="AL3"/>
+      <selection activeCell="B2" sqref="B2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1254,122 +1254,122 @@
       <c r="B1" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="31"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="34"/>
       <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="H1" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="31"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="34"/>
       <c r="M1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="N1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="31"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="34"/>
       <c r="S1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="T1" s="32" t="s">
         <v>167</v>
       </c>
-      <c r="U1" s="30"/>
-      <c r="V1" s="30"/>
-      <c r="W1" s="30"/>
-      <c r="X1" s="31"/>
+      <c r="U1" s="33"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="33"/>
+      <c r="X1" s="34"/>
       <c r="Y1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="Z1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="AA1" s="30"/>
-      <c r="AB1" s="30"/>
-      <c r="AC1" s="30"/>
-      <c r="AD1" s="31"/>
+      <c r="AA1" s="33"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="33"/>
+      <c r="AD1" s="34"/>
       <c r="AE1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="AF1" s="32" t="s">
         <v>167</v>
       </c>
-      <c r="AG1" s="30"/>
-      <c r="AH1" s="30"/>
-      <c r="AI1" s="30"/>
-      <c r="AJ1" s="31"/>
+      <c r="AG1" s="33"/>
+      <c r="AH1" s="33"/>
+      <c r="AI1" s="33"/>
+      <c r="AJ1" s="34"/>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="29">
-        <v>43872</v>
-      </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="31"/>
+      <c r="B2" s="35">
+        <v>43873</v>
+      </c>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="34"/>
       <c r="G2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="29">
-        <v>43872</v>
-      </c>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="31"/>
+      <c r="H2" s="35">
+        <v>43873</v>
+      </c>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="34"/>
       <c r="M2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="N2" s="29">
+      <c r="N2" s="35">
         <v>43873</v>
       </c>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="31"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="34"/>
       <c r="S2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="T2" s="29">
+      <c r="T2" s="35">
         <v>43873</v>
       </c>
-      <c r="U2" s="30"/>
-      <c r="V2" s="30"/>
-      <c r="W2" s="30"/>
-      <c r="X2" s="31"/>
+      <c r="U2" s="33"/>
+      <c r="V2" s="33"/>
+      <c r="W2" s="33"/>
+      <c r="X2" s="34"/>
       <c r="Y2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Z2" s="29">
+      <c r="Z2" s="35">
         <v>43873</v>
       </c>
-      <c r="AA2" s="30"/>
-      <c r="AB2" s="30"/>
-      <c r="AC2" s="30"/>
-      <c r="AD2" s="31"/>
+      <c r="AA2" s="33"/>
+      <c r="AB2" s="33"/>
+      <c r="AC2" s="33"/>
+      <c r="AD2" s="34"/>
       <c r="AE2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AF2" s="29">
+      <c r="AF2" s="35">
         <v>43873</v>
       </c>
-      <c r="AG2" s="30"/>
-      <c r="AH2" s="30"/>
-      <c r="AI2" s="30"/>
-      <c r="AJ2" s="31"/>
+      <c r="AG2" s="33"/>
+      <c r="AH2" s="33"/>
+      <c r="AI2" s="33"/>
+      <c r="AJ2" s="34"/>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -1378,122 +1378,122 @@
       <c r="B3" s="32" t="s">
         <v>204</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="31"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="34"/>
       <c r="G3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H3" s="32" t="s">
         <v>204</v>
       </c>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
-      <c r="L3" s="31"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="34"/>
       <c r="M3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="N3" s="32" t="s">
         <v>204</v>
       </c>
-      <c r="O3" s="30"/>
-      <c r="P3" s="30"/>
-      <c r="Q3" s="30"/>
-      <c r="R3" s="31"/>
+      <c r="O3" s="33"/>
+      <c r="P3" s="33"/>
+      <c r="Q3" s="33"/>
+      <c r="R3" s="34"/>
       <c r="S3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="T3" s="32" t="s">
         <v>204</v>
       </c>
-      <c r="U3" s="30"/>
-      <c r="V3" s="30"/>
-      <c r="W3" s="30"/>
-      <c r="X3" s="31"/>
+      <c r="U3" s="33"/>
+      <c r="V3" s="33"/>
+      <c r="W3" s="33"/>
+      <c r="X3" s="34"/>
       <c r="Y3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="Z3" s="32" t="s">
         <v>204</v>
       </c>
-      <c r="AA3" s="30"/>
-      <c r="AB3" s="30"/>
-      <c r="AC3" s="30"/>
-      <c r="AD3" s="31"/>
+      <c r="AA3" s="33"/>
+      <c r="AB3" s="33"/>
+      <c r="AC3" s="33"/>
+      <c r="AD3" s="34"/>
       <c r="AE3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="AF3" s="32" t="s">
         <v>204</v>
       </c>
-      <c r="AG3" s="30"/>
-      <c r="AH3" s="30"/>
-      <c r="AI3" s="30"/>
-      <c r="AJ3" s="31"/>
+      <c r="AG3" s="33"/>
+      <c r="AH3" s="33"/>
+      <c r="AI3" s="33"/>
+      <c r="AJ3" s="34"/>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="33">
+      <c r="B4" s="29">
         <v>139</v>
       </c>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="35"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="31"/>
       <c r="G4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="33">
+      <c r="H4" s="29">
         <v>140</v>
       </c>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
-      <c r="K4" s="34"/>
-      <c r="L4" s="35"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="31"/>
       <c r="M4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="N4" s="33">
+      <c r="N4" s="29">
         <v>141</v>
       </c>
-      <c r="O4" s="34"/>
-      <c r="P4" s="34"/>
-      <c r="Q4" s="34"/>
-      <c r="R4" s="35"/>
+      <c r="O4" s="30"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="30"/>
+      <c r="R4" s="31"/>
       <c r="S4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="T4" s="33">
+      <c r="T4" s="29">
         <v>142</v>
       </c>
-      <c r="U4" s="34"/>
-      <c r="V4" s="34"/>
-      <c r="W4" s="34"/>
-      <c r="X4" s="35"/>
+      <c r="U4" s="30"/>
+      <c r="V4" s="30"/>
+      <c r="W4" s="30"/>
+      <c r="X4" s="31"/>
       <c r="Y4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="Z4" s="33">
+      <c r="Z4" s="29">
         <v>143</v>
       </c>
-      <c r="AA4" s="34"/>
-      <c r="AB4" s="34"/>
-      <c r="AC4" s="34"/>
-      <c r="AD4" s="35"/>
+      <c r="AA4" s="30"/>
+      <c r="AB4" s="30"/>
+      <c r="AC4" s="30"/>
+      <c r="AD4" s="31"/>
       <c r="AE4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="AF4" s="33">
+      <c r="AF4" s="29">
         <v>144</v>
       </c>
-      <c r="AG4" s="34"/>
-      <c r="AH4" s="34"/>
-      <c r="AI4" s="34"/>
-      <c r="AJ4" s="35"/>
+      <c r="AG4" s="30"/>
+      <c r="AH4" s="30"/>
+      <c r="AI4" s="30"/>
+      <c r="AJ4" s="31"/>
     </row>
     <row r="5" spans="1:36" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
@@ -5359,6 +5359,18 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="AF2:AJ2"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="H1:L1"/>
+    <mergeCell ref="N1:R1"/>
+    <mergeCell ref="T1:X1"/>
+    <mergeCell ref="Z1:AD1"/>
+    <mergeCell ref="AF1:AJ1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="N2:R2"/>
+    <mergeCell ref="T2:X2"/>
+    <mergeCell ref="Z2:AD2"/>
     <mergeCell ref="AF4:AJ4"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="H3:L3"/>
@@ -5371,18 +5383,6 @@
     <mergeCell ref="N4:R4"/>
     <mergeCell ref="T4:X4"/>
     <mergeCell ref="Z4:AD4"/>
-    <mergeCell ref="AF2:AJ2"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="H1:L1"/>
-    <mergeCell ref="N1:R1"/>
-    <mergeCell ref="T1:X1"/>
-    <mergeCell ref="Z1:AD1"/>
-    <mergeCell ref="AF1:AJ1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="N2:R2"/>
-    <mergeCell ref="T2:X2"/>
-    <mergeCell ref="Z2:AD2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix CEI data error from NH
</commit_message>
<xml_diff>
--- a/data/tle/2020-02-12_CEI.xlsx
+++ b/data/tle/2020-02-12_CEI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrcunning/Projects/bsrte/data/tle/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67377A5C-0972-F345-B061-1B265E47C7CE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B388654B-8AEF-C044-9C40-116890C52799}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="940" windowWidth="27640" windowHeight="16000" xr2:uid="{95812F95-F459-FF47-9666-98D8637D2352}"/>
   </bookViews>
@@ -642,13 +642,13 @@
     <t>CEI</t>
   </si>
   <si>
-    <t>18,2,2,5,1,5</t>
-  </si>
-  <si>
     <t>6,2,2,1</t>
   </si>
   <si>
     <t>5,3,3,5</t>
+  </si>
+  <si>
+    <t>18,2,2,6,1,6</t>
   </si>
 </sst>
 </file>
@@ -884,19 +884,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1213,8 +1213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2B2FBFF-24C1-0B45-99C9-3C3435C2EF7C}">
   <dimension ref="A1:AJ1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="X11" sqref="X11"/>
+    <sheetView tabSelected="1" topLeftCell="I12" workbookViewId="0">
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1257,122 +1257,122 @@
       <c r="B1" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="34"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="31"/>
       <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="H1" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="34"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="31"/>
       <c r="M1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="N1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="33"/>
-      <c r="P1" s="33"/>
-      <c r="Q1" s="33"/>
-      <c r="R1" s="34"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="31"/>
       <c r="S1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="T1" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="U1" s="33"/>
-      <c r="V1" s="33"/>
-      <c r="W1" s="33"/>
-      <c r="X1" s="34"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="30"/>
+      <c r="W1" s="30"/>
+      <c r="X1" s="31"/>
       <c r="Y1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="Z1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="AA1" s="33"/>
-      <c r="AB1" s="33"/>
-      <c r="AC1" s="33"/>
-      <c r="AD1" s="34"/>
+      <c r="AA1" s="30"/>
+      <c r="AB1" s="30"/>
+      <c r="AC1" s="30"/>
+      <c r="AD1" s="31"/>
       <c r="AE1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="AF1" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="AG1" s="33"/>
-      <c r="AH1" s="33"/>
-      <c r="AI1" s="33"/>
-      <c r="AJ1" s="34"/>
+      <c r="AG1" s="30"/>
+      <c r="AH1" s="30"/>
+      <c r="AI1" s="30"/>
+      <c r="AJ1" s="31"/>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="35">
+      <c r="B2" s="29">
         <v>43873</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="34"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="31"/>
       <c r="G2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="35">
+      <c r="H2" s="29">
         <v>43873</v>
       </c>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="34"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="31"/>
       <c r="M2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="N2" s="35">
+      <c r="N2" s="29">
         <v>43873</v>
       </c>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="34"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="30"/>
+      <c r="R2" s="31"/>
       <c r="S2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="T2" s="35">
+      <c r="T2" s="29">
         <v>43873</v>
       </c>
-      <c r="U2" s="33"/>
-      <c r="V2" s="33"/>
-      <c r="W2" s="33"/>
-      <c r="X2" s="34"/>
+      <c r="U2" s="30"/>
+      <c r="V2" s="30"/>
+      <c r="W2" s="30"/>
+      <c r="X2" s="31"/>
       <c r="Y2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Z2" s="35">
+      <c r="Z2" s="29">
         <v>43873</v>
       </c>
-      <c r="AA2" s="33"/>
-      <c r="AB2" s="33"/>
-      <c r="AC2" s="33"/>
-      <c r="AD2" s="34"/>
+      <c r="AA2" s="30"/>
+      <c r="AB2" s="30"/>
+      <c r="AC2" s="30"/>
+      <c r="AD2" s="31"/>
       <c r="AE2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AF2" s="35">
+      <c r="AF2" s="29">
         <v>43873</v>
       </c>
-      <c r="AG2" s="33"/>
-      <c r="AH2" s="33"/>
-      <c r="AI2" s="33"/>
-      <c r="AJ2" s="34"/>
+      <c r="AG2" s="30"/>
+      <c r="AH2" s="30"/>
+      <c r="AI2" s="30"/>
+      <c r="AJ2" s="31"/>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -1381,122 +1381,122 @@
       <c r="B3" s="32" t="s">
         <v>202</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="34"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="31"/>
       <c r="G3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H3" s="32" t="s">
         <v>202</v>
       </c>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="34"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="31"/>
       <c r="M3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="N3" s="32" t="s">
         <v>202</v>
       </c>
-      <c r="O3" s="33"/>
-      <c r="P3" s="33"/>
-      <c r="Q3" s="33"/>
-      <c r="R3" s="34"/>
+      <c r="O3" s="30"/>
+      <c r="P3" s="30"/>
+      <c r="Q3" s="30"/>
+      <c r="R3" s="31"/>
       <c r="S3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="T3" s="32" t="s">
         <v>202</v>
       </c>
-      <c r="U3" s="33"/>
-      <c r="V3" s="33"/>
-      <c r="W3" s="33"/>
-      <c r="X3" s="34"/>
+      <c r="U3" s="30"/>
+      <c r="V3" s="30"/>
+      <c r="W3" s="30"/>
+      <c r="X3" s="31"/>
       <c r="Y3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="Z3" s="32" t="s">
         <v>202</v>
       </c>
-      <c r="AA3" s="33"/>
-      <c r="AB3" s="33"/>
-      <c r="AC3" s="33"/>
-      <c r="AD3" s="34"/>
+      <c r="AA3" s="30"/>
+      <c r="AB3" s="30"/>
+      <c r="AC3" s="30"/>
+      <c r="AD3" s="31"/>
       <c r="AE3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="AF3" s="32" t="s">
         <v>202</v>
       </c>
-      <c r="AG3" s="33"/>
-      <c r="AH3" s="33"/>
-      <c r="AI3" s="33"/>
-      <c r="AJ3" s="34"/>
+      <c r="AG3" s="30"/>
+      <c r="AH3" s="30"/>
+      <c r="AI3" s="30"/>
+      <c r="AJ3" s="31"/>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="29">
+      <c r="B4" s="33">
         <v>139</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="31"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="35"/>
       <c r="G4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="29">
+      <c r="H4" s="33">
         <v>140</v>
       </c>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="31"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="35"/>
       <c r="M4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="N4" s="29">
+      <c r="N4" s="33">
         <v>141</v>
       </c>
-      <c r="O4" s="30"/>
-      <c r="P4" s="30"/>
-      <c r="Q4" s="30"/>
-      <c r="R4" s="31"/>
+      <c r="O4" s="34"/>
+      <c r="P4" s="34"/>
+      <c r="Q4" s="34"/>
+      <c r="R4" s="35"/>
       <c r="S4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="T4" s="29">
+      <c r="T4" s="33">
         <v>142</v>
       </c>
-      <c r="U4" s="30"/>
-      <c r="V4" s="30"/>
-      <c r="W4" s="30"/>
-      <c r="X4" s="31"/>
+      <c r="U4" s="34"/>
+      <c r="V4" s="34"/>
+      <c r="W4" s="34"/>
+      <c r="X4" s="35"/>
       <c r="Y4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="Z4" s="29">
+      <c r="Z4" s="33">
         <v>143</v>
       </c>
-      <c r="AA4" s="30"/>
-      <c r="AB4" s="30"/>
-      <c r="AC4" s="30"/>
-      <c r="AD4" s="31"/>
+      <c r="AA4" s="34"/>
+      <c r="AB4" s="34"/>
+      <c r="AC4" s="34"/>
+      <c r="AD4" s="35"/>
       <c r="AE4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="AF4" s="29">
+      <c r="AF4" s="33">
         <v>144</v>
       </c>
-      <c r="AG4" s="30"/>
-      <c r="AH4" s="30"/>
-      <c r="AI4" s="30"/>
-      <c r="AJ4" s="31"/>
+      <c r="AG4" s="34"/>
+      <c r="AH4" s="34"/>
+      <c r="AI4" s="34"/>
+      <c r="AJ4" s="35"/>
     </row>
     <row r="5" spans="1:36" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
@@ -1866,7 +1866,7 @@
         <v>22</v>
       </c>
       <c r="AA8" s="12" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="AB8" s="15"/>
       <c r="AC8" s="16">
@@ -2031,7 +2031,7 @@
         <v>33</v>
       </c>
       <c r="X10" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="Y10" s="13"/>
       <c r="Z10" s="17" t="s">
@@ -3192,7 +3192,7 @@
         <v>22</v>
       </c>
       <c r="O23" s="12" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="P23" s="15"/>
       <c r="Q23" s="16">
@@ -5362,6 +5362,18 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="AF4:AJ4"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="H3:L3"/>
+    <mergeCell ref="N3:R3"/>
+    <mergeCell ref="T3:X3"/>
+    <mergeCell ref="Z3:AD3"/>
+    <mergeCell ref="AF3:AJ3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="H4:L4"/>
+    <mergeCell ref="N4:R4"/>
+    <mergeCell ref="T4:X4"/>
+    <mergeCell ref="Z4:AD4"/>
     <mergeCell ref="AF2:AJ2"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="H1:L1"/>
@@ -5374,18 +5386,6 @@
     <mergeCell ref="N2:R2"/>
     <mergeCell ref="T2:X2"/>
     <mergeCell ref="Z2:AD2"/>
-    <mergeCell ref="AF4:AJ4"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="H3:L3"/>
-    <mergeCell ref="N3:R3"/>
-    <mergeCell ref="T3:X3"/>
-    <mergeCell ref="Z3:AD3"/>
-    <mergeCell ref="AF3:AJ3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="H4:L4"/>
-    <mergeCell ref="N4:R4"/>
-    <mergeCell ref="T4:X4"/>
-    <mergeCell ref="Z4:AD4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>